<commit_message>
first version of agile lean, story and backlog
</commit_message>
<xml_diff>
--- a/Story-Mapping.xlsx
+++ b/Story-Mapping.xlsx
@@ -343,9 +343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>804600</xdr:colOff>
+      <xdr:colOff>804240</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -354,8 +354,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1210680" y="906480"/>
-          <a:ext cx="1501920" cy="677520"/>
+          <a:off x="1209960" y="906480"/>
+          <a:ext cx="1500840" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -427,9 +427,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>76680</xdr:colOff>
+      <xdr:colOff>76320</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -438,8 +438,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14025600" y="515880"/>
-          <a:ext cx="1502280" cy="662400"/>
+          <a:off x="14015160" y="515880"/>
+          <a:ext cx="1500840" cy="662040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -511,9 +511,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>815400</xdr:colOff>
+      <xdr:colOff>815040</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -522,8 +522,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1221480" y="1767960"/>
-          <a:ext cx="1501920" cy="677880"/>
+          <a:off x="1220760" y="1767960"/>
+          <a:ext cx="1500840" cy="677520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -595,9 +595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>729360</xdr:colOff>
+      <xdr:colOff>729000</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -606,8 +606,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3674880" y="936360"/>
-          <a:ext cx="1501920" cy="677520"/>
+          <a:off x="3672000" y="936360"/>
+          <a:ext cx="1501200" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -679,9 +679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>762120</xdr:colOff>
+      <xdr:colOff>761760</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -690,8 +690,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6246720" y="907560"/>
-          <a:ext cx="1502280" cy="677520"/>
+          <a:off x="6242400" y="907560"/>
+          <a:ext cx="1500840" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -763,9 +763,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>707040</xdr:colOff>
+      <xdr:colOff>706680</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -774,8 +774,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1113120" y="2850840"/>
-          <a:ext cx="1501920" cy="662760"/>
+          <a:off x="1112400" y="2850840"/>
+          <a:ext cx="1500840" cy="662400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -847,9 +847,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>788760</xdr:colOff>
+      <xdr:colOff>788400</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -858,8 +858,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3733920" y="2820960"/>
-          <a:ext cx="1502280" cy="662760"/>
+          <a:off x="3731040" y="2820960"/>
+          <a:ext cx="1501560" cy="662400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -931,9 +931,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>751680</xdr:colOff>
+      <xdr:colOff>751320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>54360</xdr:rowOff>
+      <xdr:rowOff>54000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -942,8 +942,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6237000" y="2881440"/>
-          <a:ext cx="1501560" cy="677880"/>
+          <a:off x="6232680" y="2881440"/>
+          <a:ext cx="1500120" cy="677520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1015,9 +1015,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
+      <xdr:colOff>784440</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>46080</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1026,8 +1026,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8808840" y="923040"/>
-          <a:ext cx="1501920" cy="677520"/>
+          <a:off x="8802360" y="923040"/>
+          <a:ext cx="1501200" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1099,9 +1099,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>775080</xdr:colOff>
+      <xdr:colOff>774720</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1110,8 +1110,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3719880" y="3634920"/>
-          <a:ext cx="1502640" cy="635400"/>
+          <a:off x="3717000" y="3634920"/>
+          <a:ext cx="1501920" cy="635040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1183,9 +1183,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>731520</xdr:colOff>
+      <xdr:colOff>731160</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1194,8 +1194,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6216480" y="4458240"/>
-          <a:ext cx="1501920" cy="613800"/>
+          <a:off x="6212160" y="4458240"/>
+          <a:ext cx="1500480" cy="613440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1267,9 +1267,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>741600</xdr:colOff>
+      <xdr:colOff>741240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1278,8 +1278,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6226920" y="3681720"/>
-          <a:ext cx="1501560" cy="677880"/>
+          <a:off x="6222600" y="3681720"/>
+          <a:ext cx="1500120" cy="677520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1351,9 +1351,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>764280</xdr:colOff>
+      <xdr:colOff>763920</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>35280</xdr:rowOff>
+      <xdr:rowOff>34920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1362,8 +1362,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8788680" y="2862000"/>
-          <a:ext cx="1501560" cy="678240"/>
+          <a:off x="8782200" y="2862000"/>
+          <a:ext cx="1500840" cy="677880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1426,6 +1426,426 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>70920</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>163800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>726120</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>63720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1131840" y="3668760"/>
+          <a:ext cx="1500840" cy="662040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffff00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Définir un ou plusieurs véhicules</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>91080</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>746280</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1152000" y="5286240"/>
+          <a:ext cx="1500840" cy="662040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffff00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Me connecter au back-office ?</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>105840</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>18360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>761040</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>109080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11316600" y="5238000"/>
+          <a:ext cx="1500840" cy="662040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffff00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Faire des statistiques ?</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>106200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>178920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>761400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>78840</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11316960" y="5969880"/>
+          <a:ext cx="1500840" cy="662040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffff00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Définir les prix de base par catégorie de véhicule ?</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>81000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>84240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>736200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>174600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1141920" y="6065640"/>
+          <a:ext cx="1500840" cy="662040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffff00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Gérer les comptes ?</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1436,8 +1856,8 @@
   </sheetPr>
   <dimension ref="B3:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L22" activeCellId="0" sqref="L22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1445,7 +1865,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,7 +2739,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2345,7 +2765,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
activity diagram trajet passager
</commit_message>
<xml_diff>
--- a/Story-Mapping.xlsx
+++ b/Story-Mapping.xlsx
@@ -343,9 +343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>804240</xdr:colOff>
+      <xdr:colOff>803880</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -355,7 +355,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1209960" y="906480"/>
-          <a:ext cx="1500840" cy="677160"/>
+          <a:ext cx="1500480" cy="676800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -427,9 +427,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>75960</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -439,7 +439,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14015160" y="515880"/>
-          <a:ext cx="1500840" cy="662040"/>
+          <a:ext cx="1500480" cy="661680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -511,9 +511,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>815040</xdr:colOff>
+      <xdr:colOff>814680</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>98640</xdr:rowOff>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -523,7 +523,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1220760" y="1767960"/>
-          <a:ext cx="1500840" cy="677520"/>
+          <a:ext cx="1500480" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -595,9 +595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>729000</xdr:colOff>
+      <xdr:colOff>728640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>59040</xdr:rowOff>
+      <xdr:rowOff>58680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -607,7 +607,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3672000" y="936360"/>
-          <a:ext cx="1501200" cy="677160"/>
+          <a:ext cx="1500840" cy="676800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -679,9 +679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>761760</xdr:colOff>
+      <xdr:colOff>761400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -691,7 +691,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6242400" y="907560"/>
-          <a:ext cx="1500840" cy="677160"/>
+          <a:ext cx="1500480" cy="676800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -763,9 +763,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>706680</xdr:colOff>
+      <xdr:colOff>706320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -775,7 +775,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1112400" y="2850840"/>
-          <a:ext cx="1500840" cy="662400"/>
+          <a:ext cx="1500480" cy="662040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -847,9 +847,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>788400</xdr:colOff>
+      <xdr:colOff>788040</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -859,7 +859,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3731040" y="2820960"/>
-          <a:ext cx="1501560" cy="662400"/>
+          <a:ext cx="1501200" cy="662040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -931,9 +931,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>751320</xdr:colOff>
+      <xdr:colOff>750960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -943,7 +943,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6232680" y="2881440"/>
-          <a:ext cx="1500120" cy="677520"/>
+          <a:ext cx="1499760" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1015,9 +1015,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>784440</xdr:colOff>
+      <xdr:colOff>784080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>45360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1027,7 +1027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8802360" y="923040"/>
-          <a:ext cx="1501200" cy="677160"/>
+          <a:ext cx="1500840" cy="676800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1099,9 +1099,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>774720</xdr:colOff>
+      <xdr:colOff>774360</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1111,7 +1111,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3717000" y="3634920"/>
-          <a:ext cx="1501920" cy="635040"/>
+          <a:ext cx="1501560" cy="634680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1183,9 +1183,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>731160</xdr:colOff>
+      <xdr:colOff>730800</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1195,7 +1195,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6212160" y="4458240"/>
-          <a:ext cx="1500480" cy="613440"/>
+          <a:ext cx="1500120" cy="613080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1267,9 +1267,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>741240</xdr:colOff>
+      <xdr:colOff>740880</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1279,7 +1279,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6222600" y="3681720"/>
-          <a:ext cx="1500120" cy="677520"/>
+          <a:ext cx="1499760" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1346,14 +1346,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>109080</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>98280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>763920</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:colOff>763560</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1362,8 +1362,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8782200" y="2862000"/>
-          <a:ext cx="1500840" cy="677880"/>
+          <a:off x="8782200" y="3603240"/>
+          <a:ext cx="1500480" cy="677520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1435,9 +1435,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>726120</xdr:colOff>
+      <xdr:colOff>725760</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
+      <xdr:rowOff>63360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1447,7 +1447,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1131840" y="3668760"/>
-          <a:ext cx="1500840" cy="662040"/>
+          <a:ext cx="1500480" cy="661680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1519,9 +1519,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>746280</xdr:colOff>
+      <xdr:colOff>745920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1531,7 +1531,343 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1152000" y="5286240"/>
-          <a:ext cx="1500840" cy="662040"/>
+          <a:ext cx="1500480" cy="661680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffe500"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Me connecter au back-office ?</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>105840</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>18360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>760680</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>108720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11316600" y="5238000"/>
+          <a:ext cx="1500480" cy="661680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffe500"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Faire des statistiques ?</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>106200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>178920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>761040</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>78480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11316960" y="5969880"/>
+          <a:ext cx="1500480" cy="661680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffe500"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Définir les prix de base par catégorie de véhicule ?</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>81000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>84240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>735840</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>174240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1141920" y="6065640"/>
+          <a:ext cx="1500480" cy="661680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffe500"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:srgbClr val="808080">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="333399"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Arial"/>
+            </a:rPr>
+            <a:t>Gérer les comptes ?</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>94680</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749160</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>164880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8767800" y="2801880"/>
+          <a:ext cx="1500480" cy="677520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1576,259 +1912,7 @@
               </a:uFill>
               <a:latin typeface="Arial"/>
             </a:rPr>
-            <a:t>Me connecter au back-office ?</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>761040</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11316600" y="5238000"/>
-          <a:ext cx="1500840" cy="662040"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffff00"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
-            <a:srgbClr val="808080">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="333399"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Arial"/>
-            </a:rPr>
-            <a:t>Faire des statistiques ?</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>106200</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>761400</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11316960" y="5969880"/>
-          <a:ext cx="1500840" cy="662040"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffff00"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
-            <a:srgbClr val="808080">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="333399"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Arial"/>
-            </a:rPr>
-            <a:t>Définir les prix de base par catégorie de véhicule ?</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>736200</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1141920" y="6065640"/>
-          <a:ext cx="1500840" cy="662040"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffff00"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
-            <a:srgbClr val="808080">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="333399"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Arial"/>
-            </a:rPr>
-            <a:t>Gérer les comptes ?</a:t>
+            <a:t>Voir les trajets effectués</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -1856,7 +1940,7 @@
   </sheetPr>
   <dimension ref="B3:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -1865,7 +1949,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="1" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2739,7 +2823,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2765,7 +2849,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
corrected user stories and activity diagrams
</commit_message>
<xml_diff>
--- a/Story-Mapping.xlsx
+++ b/Story-Mapping.xlsx
@@ -343,9 +343,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>803880</xdr:colOff>
+      <xdr:colOff>803520</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -355,7 +355,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1209960" y="906480"/>
-          <a:ext cx="1500480" cy="676800"/>
+          <a:ext cx="1500120" cy="676440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -427,9 +427,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>75600</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>19080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -439,7 +439,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14015160" y="515880"/>
-          <a:ext cx="1500480" cy="661680"/>
+          <a:ext cx="1500120" cy="661320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -511,9 +511,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>814680</xdr:colOff>
+      <xdr:colOff>814320</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>98280</xdr:rowOff>
+      <xdr:rowOff>97920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -523,7 +523,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1220760" y="1767960"/>
-          <a:ext cx="1500480" cy="677160"/>
+          <a:ext cx="1500120" cy="676800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -595,9 +595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>728640</xdr:colOff>
+      <xdr:colOff>728280</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>58680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -607,7 +607,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3672000" y="936360"/>
-          <a:ext cx="1500840" cy="676800"/>
+          <a:ext cx="1500480" cy="676440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -679,9 +679,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>761400</xdr:colOff>
+      <xdr:colOff>761040</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -691,7 +691,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6242400" y="907560"/>
-          <a:ext cx="1500480" cy="676800"/>
+          <a:ext cx="1500120" cy="676440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -763,9 +763,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>706320</xdr:colOff>
+      <xdr:colOff>705960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -775,7 +775,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1112400" y="2850840"/>
-          <a:ext cx="1500480" cy="662040"/>
+          <a:ext cx="1500120" cy="661680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -847,9 +847,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>788040</xdr:colOff>
+      <xdr:colOff>787680</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>168480</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -859,7 +859,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3731040" y="2820960"/>
-          <a:ext cx="1501200" cy="662040"/>
+          <a:ext cx="1500840" cy="661680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -931,9 +931,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>750960</xdr:colOff>
+      <xdr:colOff>750600</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -943,7 +943,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6232680" y="2881440"/>
-          <a:ext cx="1499760" cy="677160"/>
+          <a:ext cx="1499400" cy="676800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1015,9 +1015,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>784080</xdr:colOff>
+      <xdr:colOff>783720</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1027,7 +1027,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8802360" y="923040"/>
-          <a:ext cx="1500840" cy="676800"/>
+          <a:ext cx="1500480" cy="676440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1099,9 +1099,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>774360</xdr:colOff>
+      <xdr:colOff>774000</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1111,7 +1111,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3717000" y="3634920"/>
-          <a:ext cx="1501560" cy="634680"/>
+          <a:ext cx="1501200" cy="634320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1183,9 +1183,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>730800</xdr:colOff>
+      <xdr:colOff>730440</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>42120</xdr:rowOff>
+      <xdr:rowOff>41760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1195,7 +1195,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6212160" y="4458240"/>
-          <a:ext cx="1500120" cy="613080"/>
+          <a:ext cx="1499760" cy="612720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1267,9 +1267,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>740880</xdr:colOff>
+      <xdr:colOff>740520</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1279,7 +1279,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6222600" y="3681720"/>
-          <a:ext cx="1499760" cy="677160"/>
+          <a:ext cx="1499400" cy="676800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1351,9 +1351,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>763560</xdr:colOff>
+      <xdr:colOff>763200</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>13680</xdr:rowOff>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1363,7 +1363,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8782200" y="3603240"/>
-          <a:ext cx="1500480" cy="677520"/>
+          <a:ext cx="1500120" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1435,9 +1435,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>725760</xdr:colOff>
+      <xdr:colOff>725400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>63360</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1447,7 +1447,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1131840" y="3668760"/>
-          <a:ext cx="1500480" cy="661680"/>
+          <a:ext cx="1500120" cy="661320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1519,9 +1519,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>745920</xdr:colOff>
+      <xdr:colOff>745560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1531,7 +1531,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1152000" y="5286240"/>
-          <a:ext cx="1500480" cy="661680"/>
+          <a:ext cx="1500120" cy="661320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1576,7 +1576,7 @@
               </a:uFill>
               <a:latin typeface="Arial"/>
             </a:rPr>
-            <a:t>Me connecter au back-office ?</a:t>
+            <a:t>Me connecter au back-office</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -1597,15 +1597,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>105840</xdr:colOff>
+      <xdr:colOff>76680</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>760680</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:colOff>731160</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1614,8 +1614,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11316600" y="5238000"/>
-          <a:ext cx="1500480" cy="661680"/>
+          <a:off x="11287440" y="5324760"/>
+          <a:ext cx="1500120" cy="661320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1660,7 +1660,7 @@
               </a:uFill>
               <a:latin typeface="Arial"/>
             </a:rPr>
-            <a:t>Faire des statistiques ?</a:t>
+            <a:t>Définir les prix de base par catégorie de véhicule</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -1680,16 +1680,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>106200</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>81000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>761040</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>735480</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1698,8 +1698,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11316960" y="5969880"/>
-          <a:ext cx="1500480" cy="661680"/>
+          <a:off x="1141920" y="6065640"/>
+          <a:ext cx="1500120" cy="661320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1744,91 +1744,7 @@
               </a:uFill>
               <a:latin typeface="Arial"/>
             </a:rPr>
-            <a:t>Définir les prix de base par catégorie de véhicule ?</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>735840</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1141920" y="6065640"/>
-          <a:ext cx="1500480" cy="661680"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffe500"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
-            <a:srgbClr val="808080">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr lIns="36720" rIns="0" tIns="27360" bIns="0"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="333399"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Arial"/>
-            </a:rPr>
-            <a:t>Gérer les comptes ?</a:t>
+            <a:t>Gérer les comptes utilisateurs</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="fr-FR" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -1855,19 +1771,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>749160</xdr:colOff>
+      <xdr:colOff>748800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="CustomShape 1"/>
+        <xdr:cNvPr id="17" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8767800" y="2801880"/>
-          <a:ext cx="1500480" cy="677520"/>
+          <a:ext cx="1500120" cy="677160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1941,7 +1857,7 @@
   <dimension ref="B3:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>